<commit_message>
Refactor Task 2 and Task 3 Notebooks for Enhanced Clarity and Functionality
- Task 2:
  - Updated execution counts for code cells to reflect the correct order of execution.
  - Improved comments and print statements for better clarity on primary key analysis and uniqueness checks.
  - Enhanced output formatting for key overlap analysis and uniqueness checks.
  - Streamlined data cleaning process with clearer messaging on handling duplicates and missing values.
  - Standardized date formatting and ensured consistency in data types.
  - Clarified data integration strategy and outcomes in the final report.

- Task 3:
  - Set execution counts to null for initial cells to allow for fresh execution.
  - Removed redundant comments regarding data loading and type checks.
  - Simplified the verification of relevant columns for root cause analysis.
</commit_message>
<xml_diff>
--- a/Task_1_Cleaned_Analysis.xlsx
+++ b/Task_1_Cleaned_Analysis.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AZ101"/>
+  <dimension ref="A1:AY101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -693,11 +693,6 @@
           <t>SALES_REGION_CODE</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
-        <is>
-          <t>GENERATED_TAGS</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -913,11 +908,6 @@
       <c r="AY2" t="n">
         <v>1</v>
       </c>
-      <c r="AZ2" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1133,11 +1123,6 @@
       <c r="AY3" t="n">
         <v>1</v>
       </c>
-      <c r="AZ3" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1355,11 +1340,6 @@
       <c r="AY4" t="n">
         <v>1</v>
       </c>
-      <c r="AZ4" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1575,11 +1555,6 @@
       <c r="AY5" t="n">
         <v>1</v>
       </c>
-      <c r="AZ5" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1795,11 +1770,6 @@
       <c r="AY6" t="n">
         <v>1</v>
       </c>
-      <c r="AZ6" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2015,11 +1985,6 @@
       <c r="AY7" t="n">
         <v>1</v>
       </c>
-      <c r="AZ7" t="inlineStr">
-        <is>
-          <t>ELECTRICAL, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2235,11 +2200,6 @@
       <c r="AY8" t="n">
         <v>1</v>
       </c>
-      <c r="AZ8" t="inlineStr">
-        <is>
-          <t>ELECTRICAL, INTERIOR, SOFTWARE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2455,11 +2415,6 @@
       <c r="AY9" t="n">
         <v>1</v>
       </c>
-      <c r="AZ9" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2675,11 +2630,6 @@
       <c r="AY10" t="n">
         <v>1</v>
       </c>
-      <c r="AZ10" t="inlineStr">
-        <is>
-          <t>NOISE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2895,11 +2845,6 @@
       <c r="AY11" t="n">
         <v>1</v>
       </c>
-      <c r="AZ11" t="inlineStr">
-        <is>
-          <t>INTERIOR</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3115,11 +3060,6 @@
       <c r="AY12" t="n">
         <v>1</v>
       </c>
-      <c r="AZ12" t="inlineStr">
-        <is>
-          <t>COOLING, INTERIOR, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -3337,11 +3277,6 @@
       <c r="AY13" t="n">
         <v>1</v>
       </c>
-      <c r="AZ13" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3559,11 +3494,6 @@
       <c r="AY14" t="n">
         <v>1</v>
       </c>
-      <c r="AZ14" t="inlineStr">
-        <is>
-          <t>ENGINE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3781,11 +3711,6 @@
       <c r="AY15" t="n">
         <v>1</v>
       </c>
-      <c r="AZ15" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -4001,11 +3926,6 @@
       <c r="AY16" t="n">
         <v>1</v>
       </c>
-      <c r="AZ16" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -4221,11 +4141,6 @@
       <c r="AY17" t="n">
         <v>1</v>
       </c>
-      <c r="AZ17" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -4443,11 +4358,6 @@
       <c r="AY18" t="n">
         <v>4</v>
       </c>
-      <c r="AZ18" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -4665,11 +4575,6 @@
       <c r="AY19" t="n">
         <v>1</v>
       </c>
-      <c r="AZ19" t="inlineStr">
-        <is>
-          <t>COOLING, ELECTRICAL, ENGINE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -4887,11 +4792,6 @@
       <c r="AY20" t="n">
         <v>1</v>
       </c>
-      <c r="AZ20" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -5109,11 +5009,6 @@
       <c r="AY21" t="n">
         <v>1</v>
       </c>
-      <c r="AZ21" t="inlineStr">
-        <is>
-          <t>INTERIOR</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -5329,11 +5224,6 @@
       <c r="AY22" t="n">
         <v>1</v>
       </c>
-      <c r="AZ22" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -5551,11 +5441,6 @@
       <c r="AY23" t="n">
         <v>1</v>
       </c>
-      <c r="AZ23" t="inlineStr">
-        <is>
-          <t>COOLING, INTERIOR, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -5773,11 +5658,6 @@
       <c r="AY24" t="n">
         <v>1</v>
       </c>
-      <c r="AZ24" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -5993,11 +5873,6 @@
       <c r="AY25" t="n">
         <v>1</v>
       </c>
-      <c r="AZ25" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -6213,11 +6088,6 @@
       <c r="AY26" t="n">
         <v>1</v>
       </c>
-      <c r="AZ26" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -6433,11 +6303,6 @@
       <c r="AY27" t="n">
         <v>1</v>
       </c>
-      <c r="AZ27" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -6655,11 +6520,6 @@
       <c r="AY28" t="n">
         <v>1</v>
       </c>
-      <c r="AZ28" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -6875,11 +6735,6 @@
       <c r="AY29" t="n">
         <v>1</v>
       </c>
-      <c r="AZ29" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -7095,11 +6950,6 @@
       <c r="AY30" t="n">
         <v>1</v>
       </c>
-      <c r="AZ30" t="inlineStr">
-        <is>
-          <t>ENGINE, INTERIOR, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -7315,11 +7165,6 @@
       <c r="AY31" t="n">
         <v>1</v>
       </c>
-      <c r="AZ31" t="inlineStr">
-        <is>
-          <t>ENGINE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -7539,11 +7384,6 @@
       <c r="AY32" t="n">
         <v>1</v>
       </c>
-      <c r="AZ32" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -7759,11 +7599,6 @@
       <c r="AY33" t="n">
         <v>1</v>
       </c>
-      <c r="AZ33" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -7979,11 +7814,6 @@
       <c r="AY34" t="n">
         <v>1</v>
       </c>
-      <c r="AZ34" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -8201,11 +8031,6 @@
       <c r="AY35" t="n">
         <v>4</v>
       </c>
-      <c r="AZ35" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -8423,11 +8248,6 @@
       <c r="AY36" t="n">
         <v>1</v>
       </c>
-      <c r="AZ36" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -8643,11 +8463,6 @@
       <c r="AY37" t="n">
         <v>1</v>
       </c>
-      <c r="AZ37" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -8863,11 +8678,6 @@
       <c r="AY38" t="n">
         <v>1</v>
       </c>
-      <c r="AZ38" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -9083,11 +8893,6 @@
       <c r="AY39" t="n">
         <v>1</v>
       </c>
-      <c r="AZ39" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -9303,11 +9108,6 @@
       <c r="AY40" t="n">
         <v>1</v>
       </c>
-      <c r="AZ40" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -9523,11 +9323,6 @@
       <c r="AY41" t="n">
         <v>1</v>
       </c>
-      <c r="AZ41" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -9745,11 +9540,6 @@
       <c r="AY42" t="n">
         <v>1</v>
       </c>
-      <c r="AZ42" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -9967,11 +9757,6 @@
       <c r="AY43" t="n">
         <v>1</v>
       </c>
-      <c r="AZ43" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -10187,11 +9972,6 @@
       <c r="AY44" t="n">
         <v>1</v>
       </c>
-      <c r="AZ44" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -10407,11 +10187,6 @@
       <c r="AY45" t="n">
         <v>1</v>
       </c>
-      <c r="AZ45" t="inlineStr">
-        <is>
-          <t>INTERIOR, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -10629,11 +10404,6 @@
       <c r="AY46" t="n">
         <v>1</v>
       </c>
-      <c r="AZ46" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -10849,11 +10619,6 @@
       <c r="AY47" t="n">
         <v>1</v>
       </c>
-      <c r="AZ47" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -11069,11 +10834,6 @@
       <c r="AY48" t="n">
         <v>1</v>
       </c>
-      <c r="AZ48" t="inlineStr">
-        <is>
-          <t>ENGINE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -11291,11 +11051,6 @@
       <c r="AY49" t="n">
         <v>1</v>
       </c>
-      <c r="AZ49" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -11513,11 +11268,6 @@
       <c r="AY50" t="n">
         <v>1</v>
       </c>
-      <c r="AZ50" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -11735,11 +11485,6 @@
       <c r="AY51" t="n">
         <v>1</v>
       </c>
-      <c r="AZ51" t="inlineStr">
-        <is>
-          <t>ENGINE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -11957,11 +11702,6 @@
       <c r="AY52" t="n">
         <v>1</v>
       </c>
-      <c r="AZ52" t="inlineStr">
-        <is>
-          <t>ENGINE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -12177,11 +11917,6 @@
       <c r="AY53" t="n">
         <v>1</v>
       </c>
-      <c r="AZ53" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -12397,11 +12132,6 @@
       <c r="AY54" t="n">
         <v>1</v>
       </c>
-      <c r="AZ54" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -12617,11 +12347,6 @@
       <c r="AY55" t="n">
         <v>1</v>
       </c>
-      <c r="AZ55" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -12839,11 +12564,6 @@
       <c r="AY56" t="n">
         <v>1</v>
       </c>
-      <c r="AZ56" t="inlineStr">
-        <is>
-          <t>ENGINE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -13059,11 +12779,6 @@
       <c r="AY57" t="n">
         <v>1</v>
       </c>
-      <c r="AZ57" t="inlineStr">
-        <is>
-          <t>COOLING, ELECTRICAL, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -13283,11 +12998,6 @@
       <c r="AY58" t="n">
         <v>1</v>
       </c>
-      <c r="AZ58" t="inlineStr">
-        <is>
-          <t>COOLING</t>
-        </is>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -13505,11 +13215,6 @@
       <c r="AY59" t="n">
         <v>1</v>
       </c>
-      <c r="AZ59" t="inlineStr">
-        <is>
-          <t>COOLING, ENGINE, SOFTWARE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -13727,11 +13432,6 @@
       <c r="AY60" t="n">
         <v>1</v>
       </c>
-      <c r="AZ60" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -13949,11 +13649,6 @@
       <c r="AY61" t="n">
         <v>1</v>
       </c>
-      <c r="AZ61" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -14169,11 +13864,6 @@
       <c r="AY62" t="n">
         <v>1</v>
       </c>
-      <c r="AZ62" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -14393,11 +14083,6 @@
       <c r="AY63" t="n">
         <v>1</v>
       </c>
-      <c r="AZ63" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -14615,11 +14300,6 @@
       <c r="AY64" t="n">
         <v>1</v>
       </c>
-      <c r="AZ64" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -14837,11 +14517,6 @@
       <c r="AY65" t="n">
         <v>1</v>
       </c>
-      <c r="AZ65" t="inlineStr">
-        <is>
-          <t>COOLING</t>
-        </is>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -15057,11 +14732,6 @@
       <c r="AY66" t="n">
         <v>1</v>
       </c>
-      <c r="AZ66" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -15277,11 +14947,6 @@
       <c r="AY67" t="n">
         <v>1</v>
       </c>
-      <c r="AZ67" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -15497,11 +15162,6 @@
       <c r="AY68" t="n">
         <v>1</v>
       </c>
-      <c r="AZ68" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -15717,11 +15377,6 @@
       <c r="AY69" t="n">
         <v>1</v>
       </c>
-      <c r="AZ69" t="inlineStr">
-        <is>
-          <t>NOISE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -15939,11 +15594,6 @@
       <c r="AY70" t="n">
         <v>1</v>
       </c>
-      <c r="AZ70" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -16161,11 +15811,6 @@
       <c r="AY71" t="n">
         <v>1</v>
       </c>
-      <c r="AZ71" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -16383,11 +16028,6 @@
       <c r="AY72" t="n">
         <v>1</v>
       </c>
-      <c r="AZ72" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -16603,11 +16243,6 @@
       <c r="AY73" t="n">
         <v>1</v>
       </c>
-      <c r="AZ73" t="inlineStr">
-        <is>
-          <t>COOLING, ELECTRICAL, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -16823,11 +16458,6 @@
       <c r="AY74" t="n">
         <v>1</v>
       </c>
-      <c r="AZ74" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -17043,11 +16673,6 @@
       <c r="AY75" t="n">
         <v>1</v>
       </c>
-      <c r="AZ75" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -17265,11 +16890,6 @@
       <c r="AY76" t="n">
         <v>1</v>
       </c>
-      <c r="AZ76" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -17485,11 +17105,6 @@
       <c r="AY77" t="n">
         <v>1</v>
       </c>
-      <c r="AZ77" t="inlineStr">
-        <is>
-          <t>COOLING, ELECTRICAL, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -17705,11 +17320,6 @@
       <c r="AY78" t="n">
         <v>1</v>
       </c>
-      <c r="AZ78" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -17927,11 +17537,6 @@
       <c r="AY79" t="n">
         <v>1</v>
       </c>
-      <c r="AZ79" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -18147,11 +17752,6 @@
       <c r="AY80" t="n">
         <v>1</v>
       </c>
-      <c r="AZ80" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -18365,11 +17965,6 @@
       <c r="AY81" t="n">
         <v>4</v>
       </c>
-      <c r="AZ81" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -18587,11 +18182,6 @@
       <c r="AY82" t="n">
         <v>1</v>
       </c>
-      <c r="AZ82" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -18807,11 +18397,6 @@
       <c r="AY83" t="n">
         <v>1</v>
       </c>
-      <c r="AZ83" t="inlineStr">
-        <is>
-          <t>COOLING, ENGINE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -19027,11 +18612,6 @@
       <c r="AY84" t="n">
         <v>1</v>
       </c>
-      <c r="AZ84" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -19249,11 +18829,6 @@
       <c r="AY85" t="n">
         <v>1</v>
       </c>
-      <c r="AZ85" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -19473,11 +19048,6 @@
       <c r="AY86" t="n">
         <v>1</v>
       </c>
-      <c r="AZ86" t="inlineStr">
-        <is>
-          <t>COOLING, ELECTRICAL, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -19693,11 +19263,6 @@
       <c r="AY87" t="n">
         <v>1</v>
       </c>
-      <c r="AZ87" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -19913,11 +19478,6 @@
       <c r="AY88" t="n">
         <v>1</v>
       </c>
-      <c r="AZ88" t="inlineStr">
-        <is>
-          <t>INTERIOR, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -20133,11 +19693,6 @@
       <c r="AY89" t="n">
         <v>1</v>
       </c>
-      <c r="AZ89" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -20353,11 +19908,6 @@
       <c r="AY90" t="n">
         <v>1</v>
       </c>
-      <c r="AZ90" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -20573,11 +20123,6 @@
       <c r="AY91" t="n">
         <v>1</v>
       </c>
-      <c r="AZ91" t="inlineStr">
-        <is>
-          <t>ELECTRICAL</t>
-        </is>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -20795,11 +20340,6 @@
       <c r="AY92" t="n">
         <v>1</v>
       </c>
-      <c r="AZ92" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -21015,11 +20555,6 @@
       <c r="AY93" t="n">
         <v>1</v>
       </c>
-      <c r="AZ93" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -21235,11 +20770,6 @@
       <c r="AY94" t="n">
         <v>1</v>
       </c>
-      <c r="AZ94" t="inlineStr">
-        <is>
-          <t>COOLING, ENGINE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -21459,11 +20989,6 @@
       <c r="AY95" t="n">
         <v>1</v>
       </c>
-      <c r="AZ95" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -21679,11 +21204,6 @@
       <c r="AY96" t="n">
         <v>1</v>
       </c>
-      <c r="AZ96" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -21901,11 +21421,6 @@
       <c r="AY97" t="n">
         <v>1</v>
       </c>
-      <c r="AZ97" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -22123,11 +21638,6 @@
       <c r="AY98" t="n">
         <v>1</v>
       </c>
-      <c r="AZ98" t="inlineStr">
-        <is>
-          <t>ELECTRICAL</t>
-        </is>
-      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -22345,11 +21855,6 @@
       <c r="AY99" t="n">
         <v>1</v>
       </c>
-      <c r="AZ99" t="inlineStr">
-        <is>
-          <t>WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -22565,11 +22070,6 @@
       <c r="AY100" t="n">
         <v>1</v>
       </c>
-      <c r="AZ100" t="inlineStr">
-        <is>
-          <t>NOISE, WHEEL/TIRE</t>
-        </is>
-      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -22786,11 +22286,6 @@
       </c>
       <c r="AY101" t="n">
         <v>1</v>
-      </c>
-      <c r="AZ101" t="inlineStr">
-        <is>
-          <t>COOLING, WHEEL/TIRE</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>